<commit_message>
Rectified a couple of errors
</commit_message>
<xml_diff>
--- a/media/generated/consolidated-plan-output.xlsx
+++ b/media/generated/consolidated-plan-output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>S/No</t>
   </si>
@@ -56,6 +56,42 @@
   </si>
   <si>
     <t>Contract completion date</t>
+  </si>
+  <si>
+    <t>General Staff Salaries</t>
+  </si>
+  <si>
+    <t>UGX</t>
+  </si>
+  <si>
+    <t>GOU</t>
+  </si>
+  <si>
+    <t>Opening Domestic Bidding</t>
+  </si>
+  <si>
+    <t>Admeasurement</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>2020-09-01</t>
+  </si>
+  <si>
+    <t>2020-09-21</t>
+  </si>
+  <si>
+    <t>2020-09-28</t>
+  </si>
+  <si>
+    <t>2020-10-18</t>
+  </si>
+  <si>
+    <t>2020-10-23</t>
+  </si>
+  <si>
+    <t>2021-06-30</t>
   </si>
 </sst>
 </file>
@@ -387,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,6 +473,50 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>10000000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>